<commit_message>
kaikibunseki and cost by it
</commit_message>
<xml_diff>
--- a/実行結果/calSameImpression_twitter8_1.xlsx
+++ b/実行結果/calSameImpression_twitter8_1.xlsx
@@ -8,15 +8,51 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asatt\Documents\研究\お勉強\Programing\Go_diffusion_suppression2\実行結果\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04815251-59AC-40A3-8629-CD78ED3B906E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29EA850-0A60-45BD-A5C3-8647E9DFEEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10320" xr2:uid="{E60BD7BA-59A2-4B02-9055-7973304D468B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{E60BD7BA-59A2-4B02-9055-7973304D468B}"/>
   </bookViews>
   <sheets>
     <sheet name="calSameImpression_twitter8_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,6 +720,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>虚偽情報なし</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -745,7 +806,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -3625,6 +3685,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>総フォロワ数</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3687,6 +3802,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>拡散量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3725,6 +3895,643 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="515812032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9860017497812774E-2"/>
+                  <c:y val="0.30819444444444444"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ja-JP"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.58</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.87</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>118.06</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102.03</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>144.27000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145.93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>165.79</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>154.41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>180.27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>176.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>182.54</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>183.52</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>184.55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>196.32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>182.46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>185.62</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>208.82</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>214.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>189.31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>200.26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>191.91</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>209.08</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>208.04</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>213.22</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>204.57</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>216.89</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>196.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>193.07</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>209.16</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>214.99</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>222.68</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>191.89</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>211.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>214.67</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>224.15</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>223.05</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>222.16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>229.94</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>200.42</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>226.03</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>226.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>230.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEF0-4000-AFD4-944AA835A190}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1110174959"/>
+        <c:axId val="1110177839"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1110174959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1110177839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1110177839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1110174959"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3820,7 +4627,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4377,6 +5740,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86C0095C-6553-E2FC-5D65-CC048319E32F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -4694,10 +6098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD169B4-CB34-4266-B117-ABCCB08FA90E}">
-  <dimension ref="A1:C468"/>
+  <dimension ref="A1:K468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C468"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -5054,7 +6458,7 @@
         <v>136.28</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>33</v>
       </c>
@@ -5065,7 +6469,7 @@
         <v>97.64</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>34</v>
       </c>
@@ -5076,7 +6480,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>35</v>
       </c>
@@ -5087,7 +6491,7 @@
         <v>76.75</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>36</v>
       </c>
@@ -5098,7 +6502,7 @@
         <v>54.43</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>37</v>
       </c>
@@ -5109,7 +6513,7 @@
         <v>128.44999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>38</v>
       </c>
@@ -5120,7 +6524,7 @@
         <v>27.14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>39</v>
       </c>
@@ -5131,7 +6535,7 @@
         <v>70.48</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>40</v>
       </c>
@@ -5141,8 +6545,14 @@
       <c r="C40">
         <v>19.579999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>41</v>
       </c>
@@ -5152,8 +6562,14 @@
       <c r="C41">
         <v>103.02</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>42</v>
       </c>
@@ -5163,8 +6579,14 @@
       <c r="C42">
         <v>123.99</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>43</v>
       </c>
@@ -5175,7 +6597,7 @@
         <v>65.66</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>44</v>
       </c>
@@ -5185,8 +6607,14 @@
       <c r="C44">
         <v>8.66</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="K44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>45</v>
       </c>
@@ -5196,8 +6624,14 @@
       <c r="C45">
         <v>47.54</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>46</v>
       </c>
@@ -5208,7 +6642,7 @@
         <v>195.3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>47</v>
       </c>
@@ -5219,7 +6653,7 @@
         <v>155.4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>48</v>
       </c>
@@ -9848,6 +11282,3312 @@
       </c>
       <c r="C468">
         <v>3.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF744F9-B51A-46A5-A26D-3B061E65896A}">
+  <dimension ref="A1:D273"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>IF(D1=0,"",A1)</f>
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>IF(D1=0,"",D1)</f>
+        <v>3.27</v>
+      </c>
+      <c r="D1" cm="1">
+        <f t="array" ref="D1">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A1)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>IF(D2=0,"",A2)</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>IF(D2=0,"",D2)</f>
+        <v>7.71</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A2)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>IF(D3=0,"",A3)</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>IF(D3=0,"",D3)</f>
+        <v>92.94</v>
+      </c>
+      <c r="D3" cm="1">
+        <f t="array" ref="D3">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A3)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>92.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>IF(D4=0,"",A4)</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>IF(D4=0,"",D4)</f>
+        <v>54.79</v>
+      </c>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A4)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>54.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>IF(D5=0,"",A5)</f>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f>IF(D5=0,"",D5)</f>
+        <v>88.58</v>
+      </c>
+      <c r="D5" cm="1">
+        <f t="array" ref="D5">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A5)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>88.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>IF(D6=0,"",A6)</f>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f>IF(D6=0,"",D6)</f>
+        <v>80.41</v>
+      </c>
+      <c r="D6" cm="1">
+        <f t="array" ref="D6">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A6)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>80.41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f>IF(D7=0,"",A7)</f>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f>IF(D7=0,"",D7)</f>
+        <v>85.87</v>
+      </c>
+      <c r="D7" cm="1">
+        <f t="array" ref="D7">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A7)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>85.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>IF(D8=0,"",A8)</f>
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f>IF(D8=0,"",D8)</f>
+        <v>95.13</v>
+      </c>
+      <c r="D8" cm="1">
+        <f t="array" ref="D8">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A8)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>95.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f>IF(D9=0,"",A9)</f>
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <f>IF(D9=0,"",D9)</f>
+        <v>118.06</v>
+      </c>
+      <c r="D9" cm="1">
+        <f t="array" ref="D9">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A9)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>118.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>IF(D10=0,"",A10)</f>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <f>IF(D10=0,"",D10)</f>
+        <v>86.2</v>
+      </c>
+      <c r="D10" cm="1">
+        <f t="array" ref="D10">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A10)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>IF(D11=0,"",A11)</f>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f>IF(D11=0,"",D11)</f>
+        <v>102.03</v>
+      </c>
+      <c r="D11" cm="1">
+        <f t="array" ref="D11">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A11)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>102.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <f>IF(D12=0,"",A12)</f>
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <f>IF(D12=0,"",D12)</f>
+        <v>144.27000000000001</v>
+      </c>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A12)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>144.27000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f>IF(D13=0,"",A13)</f>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f>IF(D13=0,"",D13)</f>
+        <v>145.93</v>
+      </c>
+      <c r="D13" cm="1">
+        <f t="array" ref="D13">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A13)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>145.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f>IF(D14=0,"",A14)</f>
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <f>IF(D14=0,"",D14)</f>
+        <v>165.79</v>
+      </c>
+      <c r="D14" cm="1">
+        <f t="array" ref="D14">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A14)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>165.79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <f>IF(D15=0,"",A15)</f>
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <f>IF(D15=0,"",D15)</f>
+        <v>154.41</v>
+      </c>
+      <c r="D15" cm="1">
+        <f t="array" ref="D15">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A15)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>154.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <f>IF(D16=0,"",A16)</f>
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <f>IF(D16=0,"",D16)</f>
+        <v>180.27</v>
+      </c>
+      <c r="D16" cm="1">
+        <f t="array" ref="D16">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A16)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>180.27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <f>IF(D17=0,"",A17)</f>
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <f>IF(D17=0,"",D17)</f>
+        <v>160.91999999999999</v>
+      </c>
+      <c r="D17" cm="1">
+        <f t="array" ref="D17">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A17)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>160.91999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <f>IF(D18=0,"",A18)</f>
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <f>IF(D18=0,"",D18)</f>
+        <v>176.54</v>
+      </c>
+      <c r="D18" cm="1">
+        <f t="array" ref="D18">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A18)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>176.54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <f>IF(D19=0,"",A19)</f>
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <f>IF(D19=0,"",D19)</f>
+        <v>182.54</v>
+      </c>
+      <c r="D19" cm="1">
+        <f t="array" ref="D19">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A19)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>182.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <f>IF(D20=0,"",A20)</f>
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <f>IF(D20=0,"",D20)</f>
+        <v>183.52</v>
+      </c>
+      <c r="D20" cm="1">
+        <f t="array" ref="D20">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A20)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>183.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <f>IF(D21=0,"",A21)</f>
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <f>IF(D21=0,"",D21)</f>
+        <v>184.55</v>
+      </c>
+      <c r="D21" cm="1">
+        <f t="array" ref="D21">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A21)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>184.55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <f>IF(D22=0,"",A22)</f>
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <f>IF(D22=0,"",D22)</f>
+        <v>196.32</v>
+      </c>
+      <c r="D22" cm="1">
+        <f t="array" ref="D22">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A22)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>196.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <f>IF(D23=0,"",A23)</f>
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <f>IF(D23=0,"",D23)</f>
+        <v>182.46</v>
+      </c>
+      <c r="D23" cm="1">
+        <f t="array" ref="D23">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A23)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>182.46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <f>IF(D24=0,"",A24)</f>
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <f>IF(D24=0,"",D24)</f>
+        <v>185.62</v>
+      </c>
+      <c r="D24" cm="1">
+        <f t="array" ref="D24">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A24)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>185.62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <f>IF(D25=0,"",A25)</f>
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <f>IF(D25=0,"",D25)</f>
+        <v>208.82</v>
+      </c>
+      <c r="D25" cm="1">
+        <f t="array" ref="D25">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A25)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>208.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <f>IF(D26=0,"",A26)</f>
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <f>IF(D26=0,"",D26)</f>
+        <v>214.3</v>
+      </c>
+      <c r="D26" cm="1">
+        <f t="array" ref="D26">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A26)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>214.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <f>IF(D27=0,"",A27)</f>
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <f>IF(D27=0,"",D27)</f>
+        <v>189.31</v>
+      </c>
+      <c r="D27" cm="1">
+        <f t="array" ref="D27">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A27)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>189.31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <f>IF(D28=0,"",A28)</f>
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <f>IF(D28=0,"",D28)</f>
+        <v>200.26</v>
+      </c>
+      <c r="D28" cm="1">
+        <f t="array" ref="D28">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A28)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>200.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <f>IF(D29=0,"",A29)</f>
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <f>IF(D29=0,"",D29)</f>
+        <v>191.91</v>
+      </c>
+      <c r="D29" cm="1">
+        <f t="array" ref="D29">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A29)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>191.91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <f>IF(D30=0,"",A30)</f>
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <f>IF(D30=0,"",D30)</f>
+        <v>209.08</v>
+      </c>
+      <c r="D30" cm="1">
+        <f t="array" ref="D30">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A30)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>209.08</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <f>IF(D31=0,"",A31)</f>
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <f>IF(D31=0,"",D31)</f>
+        <v>208.04</v>
+      </c>
+      <c r="D31" cm="1">
+        <f t="array" ref="D31">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A31)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>208.04</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <f>IF(D32=0,"",A32)</f>
+        <v>36</v>
+      </c>
+      <c r="C32">
+        <f>IF(D32=0,"",D32)</f>
+        <v>213.22</v>
+      </c>
+      <c r="D32" cm="1">
+        <f t="array" ref="D32">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A32)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>213.22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <f>IF(D33=0,"",A33)</f>
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <f>IF(D33=0,"",D33)</f>
+        <v>204.57</v>
+      </c>
+      <c r="D33" cm="1">
+        <f t="array" ref="D33">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A33)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>204.57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <f>IF(D34=0,"",A34)</f>
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <f>IF(D34=0,"",D34)</f>
+        <v>216.89</v>
+      </c>
+      <c r="D34" cm="1">
+        <f t="array" ref="D34">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A34)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>216.89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <f>IF(D35=0,"",A35)</f>
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <f>IF(D35=0,"",D35)</f>
+        <v>196.2</v>
+      </c>
+      <c r="D35" cm="1">
+        <f t="array" ref="D35">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A35)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>196.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <f>IF(D36=0,"",A36)</f>
+        <v>40</v>
+      </c>
+      <c r="C36">
+        <f>IF(D36=0,"",D36)</f>
+        <v>193.07</v>
+      </c>
+      <c r="D36" cm="1">
+        <f t="array" ref="D36">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A36)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>193.07</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <f>IF(D37=0,"",A37)</f>
+        <v>41</v>
+      </c>
+      <c r="C37">
+        <f>IF(D37=0,"",D37)</f>
+        <v>209.16</v>
+      </c>
+      <c r="D37" cm="1">
+        <f t="array" ref="D37">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A37)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>209.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>43</v>
+      </c>
+      <c r="B38">
+        <f>IF(D38=0,"",A38)</f>
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <f>IF(D38=0,"",D38)</f>
+        <v>214.99</v>
+      </c>
+      <c r="D38" cm="1">
+        <f t="array" ref="D38">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A38)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>214.99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <f>IF(D39=0,"",A39)</f>
+        <v>44</v>
+      </c>
+      <c r="C39">
+        <f>IF(D39=0,"",D39)</f>
+        <v>222.68</v>
+      </c>
+      <c r="D39" cm="1">
+        <f t="array" ref="D39">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A39)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>222.68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <f>IF(D40=0,"",A40)</f>
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <f>IF(D40=0,"",D40)</f>
+        <v>191.89</v>
+      </c>
+      <c r="D40" cm="1">
+        <f t="array" ref="D40">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A40)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>191.89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>47</v>
+      </c>
+      <c r="B41">
+        <f>IF(D41=0,"",A41)</f>
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <f>IF(D41=0,"",D41)</f>
+        <v>211.7</v>
+      </c>
+      <c r="D41" cm="1">
+        <f t="array" ref="D41">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A41)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>211.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <f>IF(D42=0,"",A42)</f>
+        <v>51</v>
+      </c>
+      <c r="C42">
+        <f>IF(D42=0,"",D42)</f>
+        <v>214.67</v>
+      </c>
+      <c r="D42" cm="1">
+        <f t="array" ref="D42">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A42)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>214.67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <f>IF(D43=0,"",A43)</f>
+        <v>52</v>
+      </c>
+      <c r="C43">
+        <f>IF(D43=0,"",D43)</f>
+        <v>224.15</v>
+      </c>
+      <c r="D43" cm="1">
+        <f t="array" ref="D43">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A43)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>224.15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <f>IF(D44=0,"",A44)</f>
+        <v>53</v>
+      </c>
+      <c r="C44">
+        <f>IF(D44=0,"",D44)</f>
+        <v>223.05</v>
+      </c>
+      <c r="D44" cm="1">
+        <f t="array" ref="D44">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A44)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>223.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <f>IF(D45=0,"",A45)</f>
+        <v>54</v>
+      </c>
+      <c r="C45">
+        <f>IF(D45=0,"",D45)</f>
+        <v>222.16</v>
+      </c>
+      <c r="D45" cm="1">
+        <f t="array" ref="D45">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A45)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>222.16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <f>IF(D46=0,"",A46)</f>
+        <v>55</v>
+      </c>
+      <c r="C46">
+        <f>IF(D46=0,"",D46)</f>
+        <v>229.94</v>
+      </c>
+      <c r="D46" cm="1">
+        <f t="array" ref="D46">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A46)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>229.94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <f>IF(D47=0,"",A47)</f>
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <f>IF(D47=0,"",D47)</f>
+        <v>200.42</v>
+      </c>
+      <c r="D47" cm="1">
+        <f t="array" ref="D47">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A47)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>200.42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>62</v>
+      </c>
+      <c r="B48">
+        <f>IF(D48=0,"",A48)</f>
+        <v>62</v>
+      </c>
+      <c r="C48">
+        <f>IF(D48=0,"",D48)</f>
+        <v>226.03</v>
+      </c>
+      <c r="D48" cm="1">
+        <f t="array" ref="D48">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A48)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>226.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>66</v>
+      </c>
+      <c r="B49">
+        <f>IF(D49=0,"",A49)</f>
+        <v>66</v>
+      </c>
+      <c r="C49">
+        <f>IF(D49=0,"",D49)</f>
+        <v>226.9</v>
+      </c>
+      <c r="D49" cm="1">
+        <f t="array" ref="D49">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A49)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>226.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>68</v>
+      </c>
+      <c r="B50">
+        <f>IF(D50=0,"",A50)</f>
+        <v>68</v>
+      </c>
+      <c r="C50">
+        <f>IF(D50=0,"",D50)</f>
+        <v>230.32</v>
+      </c>
+      <c r="D50" cm="1">
+        <f t="array" ref="D50">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A50)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>230.32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>72</v>
+      </c>
+      <c r="B51">
+        <f>IF(D51=0,"",A51)</f>
+        <v>72</v>
+      </c>
+      <c r="C51">
+        <f>IF(D51=0,"",D51)</f>
+        <v>209.31</v>
+      </c>
+      <c r="D51" cm="1">
+        <f t="array" ref="D51">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A51)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>209.31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>74</v>
+      </c>
+      <c r="B52">
+        <f>IF(D52=0,"",A52)</f>
+        <v>74</v>
+      </c>
+      <c r="C52">
+        <f>IF(D52=0,"",D52)</f>
+        <v>233.45</v>
+      </c>
+      <c r="D52" cm="1">
+        <f t="array" ref="D52">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A52)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>233.45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>75</v>
+      </c>
+      <c r="B53">
+        <f>IF(D53=0,"",A53)</f>
+        <v>75</v>
+      </c>
+      <c r="C53">
+        <f>IF(D53=0,"",D53)</f>
+        <v>224.8</v>
+      </c>
+      <c r="D53" cm="1">
+        <f t="array" ref="D53">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A53)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>224.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>84</v>
+      </c>
+      <c r="B54">
+        <f>IF(D54=0,"",A54)</f>
+        <v>84</v>
+      </c>
+      <c r="C54">
+        <f>IF(D54=0,"",D54)</f>
+        <v>218.33</v>
+      </c>
+      <c r="D54" cm="1">
+        <f t="array" ref="D54">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A54)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>218.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <f>IF(D55=0,"",A55)</f>
+        <v>86</v>
+      </c>
+      <c r="C55">
+        <f>IF(D55=0,"",D55)</f>
+        <v>170.86</v>
+      </c>
+      <c r="D55" cm="1">
+        <f t="array" ref="D55">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A55)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>170.86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>91</v>
+      </c>
+      <c r="B56">
+        <f>IF(D56=0,"",A56)</f>
+        <v>91</v>
+      </c>
+      <c r="C56">
+        <f>IF(D56=0,"",D56)</f>
+        <v>187.29</v>
+      </c>
+      <c r="D56" cm="1">
+        <f t="array" ref="D56">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A56)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>187.29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>94</v>
+      </c>
+      <c r="B57">
+        <f>IF(D57=0,"",A57)</f>
+        <v>94</v>
+      </c>
+      <c r="C57">
+        <f>IF(D57=0,"",D57)</f>
+        <v>227.83</v>
+      </c>
+      <c r="D57" cm="1">
+        <f t="array" ref="D57">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A57)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>227.83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>97</v>
+      </c>
+      <c r="B58">
+        <f>IF(D58=0,"",A58)</f>
+        <v>97</v>
+      </c>
+      <c r="C58">
+        <f>IF(D58=0,"",D58)</f>
+        <v>231.78</v>
+      </c>
+      <c r="D58" cm="1">
+        <f t="array" ref="D58">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A58)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>231.78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>105</v>
+      </c>
+      <c r="B59">
+        <f>IF(D59=0,"",A59)</f>
+        <v>105</v>
+      </c>
+      <c r="C59">
+        <f>IF(D59=0,"",D59)</f>
+        <v>184.12</v>
+      </c>
+      <c r="D59" cm="1">
+        <f t="array" ref="D59">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A59)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>184.12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>106</v>
+      </c>
+      <c r="B60">
+        <f>IF(D60=0,"",A60)</f>
+        <v>106</v>
+      </c>
+      <c r="C60">
+        <f>IF(D60=0,"",D60)</f>
+        <v>197.47</v>
+      </c>
+      <c r="D60" cm="1">
+        <f t="array" ref="D60">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A60)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>197.47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>108</v>
+      </c>
+      <c r="B61">
+        <f>IF(D61=0,"",A61)</f>
+        <v>108</v>
+      </c>
+      <c r="C61">
+        <f>IF(D61=0,"",D61)</f>
+        <v>216.15</v>
+      </c>
+      <c r="D61" cm="1">
+        <f t="array" ref="D61">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A61)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>216.15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>109</v>
+      </c>
+      <c r="B62">
+        <f>IF(D62=0,"",A62)</f>
+        <v>109</v>
+      </c>
+      <c r="C62">
+        <f>IF(D62=0,"",D62)</f>
+        <v>230.35</v>
+      </c>
+      <c r="D62" cm="1">
+        <f t="array" ref="D62">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A62)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>230.35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>120</v>
+      </c>
+      <c r="B63">
+        <f>IF(D63=0,"",A63)</f>
+        <v>120</v>
+      </c>
+      <c r="C63">
+        <f>IF(D63=0,"",D63)</f>
+        <v>204.62</v>
+      </c>
+      <c r="D63" cm="1">
+        <f t="array" ref="D63">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A63)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>204.62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>121</v>
+      </c>
+      <c r="B64">
+        <f>IF(D64=0,"",A64)</f>
+        <v>121</v>
+      </c>
+      <c r="C64">
+        <f>IF(D64=0,"",D64)</f>
+        <v>219.41</v>
+      </c>
+      <c r="D64" cm="1">
+        <f t="array" ref="D64">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A64)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>219.41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>122</v>
+      </c>
+      <c r="B65" t="str">
+        <f>IF(D65=0,"",A65)</f>
+        <v/>
+      </c>
+      <c r="C65" t="str">
+        <f>IF(D65=0,"",D65)</f>
+        <v/>
+      </c>
+      <c r="D65" cm="1">
+        <f t="array" ref="D65">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A65)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>123</v>
+      </c>
+      <c r="B66" t="str">
+        <f>IF(D66=0,"",A66)</f>
+        <v/>
+      </c>
+      <c r="C66" t="str">
+        <f>IF(D66=0,"",D66)</f>
+        <v/>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A66)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>124</v>
+      </c>
+      <c r="B67" t="str">
+        <f>IF(D67=0,"",A67)</f>
+        <v/>
+      </c>
+      <c r="C67" t="str">
+        <f>IF(D67=0,"",D67)</f>
+        <v/>
+      </c>
+      <c r="D67" cm="1">
+        <f t="array" ref="D67">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A67)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>125</v>
+      </c>
+      <c r="B68" t="str">
+        <f>IF(D68=0,"",A68)</f>
+        <v/>
+      </c>
+      <c r="C68" t="str">
+        <f>IF(D68=0,"",D68)</f>
+        <v/>
+      </c>
+      <c r="D68" cm="1">
+        <f t="array" ref="D68">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A68)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>126</v>
+      </c>
+      <c r="B69" t="str">
+        <f>IF(D69=0,"",A69)</f>
+        <v/>
+      </c>
+      <c r="C69" t="str">
+        <f>IF(D69=0,"",D69)</f>
+        <v/>
+      </c>
+      <c r="D69" cm="1">
+        <f t="array" ref="D69">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A69)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>127</v>
+      </c>
+      <c r="B70" t="str">
+        <f>IF(D70=0,"",A70)</f>
+        <v/>
+      </c>
+      <c r="C70" t="str">
+        <f>IF(D70=0,"",D70)</f>
+        <v/>
+      </c>
+      <c r="D70" cm="1">
+        <f t="array" ref="D70">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A70)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>128</v>
+      </c>
+      <c r="B71" t="str">
+        <f>IF(D71=0,"",A71)</f>
+        <v/>
+      </c>
+      <c r="C71" t="str">
+        <f>IF(D71=0,"",D71)</f>
+        <v/>
+      </c>
+      <c r="D71" cm="1">
+        <f t="array" ref="D71">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A71)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>129</v>
+      </c>
+      <c r="B72" t="str">
+        <f>IF(D72=0,"",A72)</f>
+        <v/>
+      </c>
+      <c r="C72" t="str">
+        <f>IF(D72=0,"",D72)</f>
+        <v/>
+      </c>
+      <c r="D72" cm="1">
+        <f t="array" ref="D72">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A72)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>130</v>
+      </c>
+      <c r="B73" t="str">
+        <f>IF(D73=0,"",A73)</f>
+        <v/>
+      </c>
+      <c r="C73" t="str">
+        <f>IF(D73=0,"",D73)</f>
+        <v/>
+      </c>
+      <c r="D73" cm="1">
+        <f t="array" ref="D73">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A73)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>131</v>
+      </c>
+      <c r="B74" t="str">
+        <f>IF(D74=0,"",A74)</f>
+        <v/>
+      </c>
+      <c r="C74" t="str">
+        <f>IF(D74=0,"",D74)</f>
+        <v/>
+      </c>
+      <c r="D74" cm="1">
+        <f t="array" ref="D74">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A74)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>132</v>
+      </c>
+      <c r="B75" t="str">
+        <f>IF(D75=0,"",A75)</f>
+        <v/>
+      </c>
+      <c r="C75" t="str">
+        <f>IF(D75=0,"",D75)</f>
+        <v/>
+      </c>
+      <c r="D75" cm="1">
+        <f t="array" ref="D75">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A75)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>133</v>
+      </c>
+      <c r="B76" t="str">
+        <f>IF(D76=0,"",A76)</f>
+        <v/>
+      </c>
+      <c r="C76" t="str">
+        <f>IF(D76=0,"",D76)</f>
+        <v/>
+      </c>
+      <c r="D76" cm="1">
+        <f t="array" ref="D76">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A76)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>134</v>
+      </c>
+      <c r="B77" t="str">
+        <f>IF(D77=0,"",A77)</f>
+        <v/>
+      </c>
+      <c r="C77" t="str">
+        <f>IF(D77=0,"",D77)</f>
+        <v/>
+      </c>
+      <c r="D77" cm="1">
+        <f t="array" ref="D77">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A77)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>135</v>
+      </c>
+      <c r="B78" t="str">
+        <f>IF(D78=0,"",A78)</f>
+        <v/>
+      </c>
+      <c r="C78" t="str">
+        <f>IF(D78=0,"",D78)</f>
+        <v/>
+      </c>
+      <c r="D78" cm="1">
+        <f t="array" ref="D78">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A78)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>136</v>
+      </c>
+      <c r="B79" t="str">
+        <f>IF(D79=0,"",A79)</f>
+        <v/>
+      </c>
+      <c r="C79" t="str">
+        <f>IF(D79=0,"",D79)</f>
+        <v/>
+      </c>
+      <c r="D79" cm="1">
+        <f t="array" ref="D79">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A79)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>137</v>
+      </c>
+      <c r="C80" t="str">
+        <f>IF(D80=0,"",D80)</f>
+        <v/>
+      </c>
+      <c r="D80" cm="1">
+        <f t="array" ref="D80">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A80)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>138</v>
+      </c>
+      <c r="C81" t="str">
+        <f>IF(D81=0,"",D81)</f>
+        <v/>
+      </c>
+      <c r="D81" cm="1">
+        <f t="array" ref="D81">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A81)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>139</v>
+      </c>
+      <c r="C82" t="str">
+        <f>IF(D82=0,"",D82)</f>
+        <v/>
+      </c>
+      <c r="D82" cm="1">
+        <f t="array" ref="D82">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A82)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>140</v>
+      </c>
+      <c r="C83" t="str">
+        <f>IF(D83=0,"",D83)</f>
+        <v/>
+      </c>
+      <c r="D83" cm="1">
+        <f t="array" ref="D83">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A83)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>141</v>
+      </c>
+      <c r="C84" t="str">
+        <f>IF(D84=0,"",D84)</f>
+        <v/>
+      </c>
+      <c r="D84" cm="1">
+        <f t="array" ref="D84">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A84)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>142</v>
+      </c>
+      <c r="C85" t="str">
+        <f>IF(D85=0,"",D85)</f>
+        <v/>
+      </c>
+      <c r="D85" cm="1">
+        <f t="array" ref="D85">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A85)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>143</v>
+      </c>
+      <c r="C86" t="str">
+        <f>IF(D86=0,"",D86)</f>
+        <v/>
+      </c>
+      <c r="D86" cm="1">
+        <f t="array" ref="D86">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A86)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>144</v>
+      </c>
+      <c r="C87" t="str">
+        <f>IF(D87=0,"",D87)</f>
+        <v/>
+      </c>
+      <c r="D87" cm="1">
+        <f t="array" ref="D87">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A87)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>145</v>
+      </c>
+      <c r="C88" t="str">
+        <f>IF(D88=0,"",D88)</f>
+        <v/>
+      </c>
+      <c r="D88" cm="1">
+        <f t="array" ref="D88">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A88)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>146</v>
+      </c>
+      <c r="C89" t="str">
+        <f>IF(D89=0,"",D89)</f>
+        <v/>
+      </c>
+      <c r="D89" cm="1">
+        <f t="array" ref="D89">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A89)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>147</v>
+      </c>
+      <c r="C90" t="str">
+        <f>IF(D90=0,"",D90)</f>
+        <v/>
+      </c>
+      <c r="D90" cm="1">
+        <f t="array" ref="D90">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A90)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>148</v>
+      </c>
+      <c r="C91" t="str">
+        <f>IF(D91=0,"",D91)</f>
+        <v/>
+      </c>
+      <c r="D91" cm="1">
+        <f t="array" ref="D91">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A91)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>149</v>
+      </c>
+      <c r="C92" t="str">
+        <f>IF(D92=0,"",D92)</f>
+        <v/>
+      </c>
+      <c r="D92" cm="1">
+        <f t="array" ref="D92">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A92)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>150</v>
+      </c>
+      <c r="C93" t="str">
+        <f>IF(D93=0,"",D93)</f>
+        <v/>
+      </c>
+      <c r="D93" cm="1">
+        <f t="array" ref="D93">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A93)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>151</v>
+      </c>
+      <c r="C94" t="str">
+        <f>IF(D94=0,"",D94)</f>
+        <v/>
+      </c>
+      <c r="D94" cm="1">
+        <f t="array" ref="D94">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A94)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>152</v>
+      </c>
+      <c r="C95" t="str">
+        <f>IF(D95=0,"",D95)</f>
+        <v/>
+      </c>
+      <c r="D95" cm="1">
+        <f t="array" ref="D95">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A95)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>153</v>
+      </c>
+      <c r="C96" t="str">
+        <f>IF(D96=0,"",D96)</f>
+        <v/>
+      </c>
+      <c r="D96" cm="1">
+        <f t="array" ref="D96">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A96)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>154</v>
+      </c>
+      <c r="C97" t="str">
+        <f>IF(D97=0,"",D97)</f>
+        <v/>
+      </c>
+      <c r="D97" cm="1">
+        <f t="array" ref="D97">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A97)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>155</v>
+      </c>
+      <c r="C98" t="str">
+        <f>IF(D98=0,"",D98)</f>
+        <v/>
+      </c>
+      <c r="D98" cm="1">
+        <f t="array" ref="D98">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A98)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>156</v>
+      </c>
+      <c r="C99" t="str">
+        <f>IF(D99=0,"",D99)</f>
+        <v/>
+      </c>
+      <c r="D99" cm="1">
+        <f t="array" ref="D99">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A99)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>157</v>
+      </c>
+      <c r="C100" t="str">
+        <f>IF(D100=0,"",D100)</f>
+        <v/>
+      </c>
+      <c r="D100" cm="1">
+        <f t="array" ref="D100">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A100)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>158</v>
+      </c>
+      <c r="C101" t="str">
+        <f>IF(D101=0,"",D101)</f>
+        <v/>
+      </c>
+      <c r="D101" cm="1">
+        <f t="array" ref="D101">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A101)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102">
+        <v>159</v>
+      </c>
+      <c r="C102" t="str">
+        <f>IF(D102=0,"",D102)</f>
+        <v/>
+      </c>
+      <c r="D102" cm="1">
+        <f t="array" ref="D102">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A102)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103">
+        <v>160</v>
+      </c>
+      <c r="C103" t="str">
+        <f>IF(D103=0,"",D103)</f>
+        <v/>
+      </c>
+      <c r="D103" cm="1">
+        <f t="array" ref="D103">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A103)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
+        <v>161</v>
+      </c>
+      <c r="C104" t="str">
+        <f>IF(D104=0,"",D104)</f>
+        <v/>
+      </c>
+      <c r="D104" cm="1">
+        <f t="array" ref="D104">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A104)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
+        <v>162</v>
+      </c>
+      <c r="C105" t="str">
+        <f>IF(D105=0,"",D105)</f>
+        <v/>
+      </c>
+      <c r="D105" cm="1">
+        <f t="array" ref="D105">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A105)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
+        <v>163</v>
+      </c>
+      <c r="C106" t="str">
+        <f>IF(D106=0,"",D106)</f>
+        <v/>
+      </c>
+      <c r="D106" cm="1">
+        <f t="array" ref="D106">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A106)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
+        <v>164</v>
+      </c>
+      <c r="C107" t="str">
+        <f>IF(D107=0,"",D107)</f>
+        <v/>
+      </c>
+      <c r="D107" cm="1">
+        <f t="array" ref="D107">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A107)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
+        <v>165</v>
+      </c>
+      <c r="C108" t="str">
+        <f>IF(D108=0,"",D108)</f>
+        <v/>
+      </c>
+      <c r="D108" cm="1">
+        <f t="array" ref="D108">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A108)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109">
+        <v>166</v>
+      </c>
+      <c r="C109" t="str">
+        <f>IF(D109=0,"",D109)</f>
+        <v/>
+      </c>
+      <c r="D109" cm="1">
+        <f t="array" ref="D109">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A109)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110">
+        <v>167</v>
+      </c>
+      <c r="C110" t="str">
+        <f>IF(D110=0,"",D110)</f>
+        <v/>
+      </c>
+      <c r="D110" cm="1">
+        <f t="array" ref="D110">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A110)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
+        <v>168</v>
+      </c>
+      <c r="C111" t="str">
+        <f>IF(D111=0,"",D111)</f>
+        <v/>
+      </c>
+      <c r="D111" cm="1">
+        <f t="array" ref="D111">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A111)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
+        <v>169</v>
+      </c>
+      <c r="C112" t="str">
+        <f>IF(D112=0,"",D112)</f>
+        <v/>
+      </c>
+      <c r="D112" cm="1">
+        <f t="array" ref="D112">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A112)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <v>170</v>
+      </c>
+      <c r="C113" t="str">
+        <f>IF(D113=0,"",D113)</f>
+        <v/>
+      </c>
+      <c r="D113" cm="1">
+        <f t="array" ref="D113">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A113)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <v>171</v>
+      </c>
+      <c r="C114" t="str">
+        <f>IF(D114=0,"",D114)</f>
+        <v/>
+      </c>
+      <c r="D114" cm="1">
+        <f t="array" ref="D114">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A114)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>172</v>
+      </c>
+      <c r="C115" t="str">
+        <f>IF(D115=0,"",D115)</f>
+        <v/>
+      </c>
+      <c r="D115" cm="1">
+        <f t="array" ref="D115">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A115)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <v>173</v>
+      </c>
+      <c r="C116" t="str">
+        <f>IF(D116=0,"",D116)</f>
+        <v/>
+      </c>
+      <c r="D116" cm="1">
+        <f t="array" ref="D116">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A116)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <v>174</v>
+      </c>
+      <c r="C117" t="str">
+        <f>IF(D117=0,"",D117)</f>
+        <v/>
+      </c>
+      <c r="D117" cm="1">
+        <f t="array" ref="D117">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A117)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <v>175</v>
+      </c>
+      <c r="C118" t="str">
+        <f>IF(D118=0,"",D118)</f>
+        <v/>
+      </c>
+      <c r="D118" cm="1">
+        <f t="array" ref="D118">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A118)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
+        <v>176</v>
+      </c>
+      <c r="C119" t="str">
+        <f>IF(D119=0,"",D119)</f>
+        <v/>
+      </c>
+      <c r="D119" cm="1">
+        <f t="array" ref="D119">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A119)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
+        <v>177</v>
+      </c>
+      <c r="C120" t="str">
+        <f>IF(D120=0,"",D120)</f>
+        <v/>
+      </c>
+      <c r="D120" cm="1">
+        <f t="array" ref="D120">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A120)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
+        <v>178</v>
+      </c>
+      <c r="C121" t="str">
+        <f>IF(D121=0,"",D121)</f>
+        <v/>
+      </c>
+      <c r="D121" cm="1">
+        <f t="array" ref="D121">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A121)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
+        <v>179</v>
+      </c>
+      <c r="C122" t="str">
+        <f>IF(D122=0,"",D122)</f>
+        <v/>
+      </c>
+      <c r="D122" cm="1">
+        <f t="array" ref="D122">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A122)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123">
+        <v>180</v>
+      </c>
+      <c r="C123" t="str">
+        <f>IF(D123=0,"",D123)</f>
+        <v/>
+      </c>
+      <c r="D123" cm="1">
+        <f t="array" ref="D123">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A123)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124">
+        <v>181</v>
+      </c>
+      <c r="C124" t="str">
+        <f>IF(D124=0,"",D124)</f>
+        <v/>
+      </c>
+      <c r="D124" cm="1">
+        <f t="array" ref="D124">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A124)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125">
+        <v>182</v>
+      </c>
+      <c r="C125" t="str">
+        <f>IF(D125=0,"",D125)</f>
+        <v/>
+      </c>
+      <c r="D125" cm="1">
+        <f t="array" ref="D125">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A125)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126">
+        <v>183</v>
+      </c>
+      <c r="C126" t="str">
+        <f>IF(D126=0,"",D126)</f>
+        <v/>
+      </c>
+      <c r="D126" cm="1">
+        <f t="array" ref="D126">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A126)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127">
+        <v>184</v>
+      </c>
+      <c r="C127" t="str">
+        <f>IF(D127=0,"",D127)</f>
+        <v/>
+      </c>
+      <c r="D127" cm="1">
+        <f t="array" ref="D127">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A127)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128">
+        <v>185</v>
+      </c>
+      <c r="C128" t="str">
+        <f>IF(D128=0,"",D128)</f>
+        <v/>
+      </c>
+      <c r="D128" cm="1">
+        <f t="array" ref="D128">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A128)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129">
+        <v>186</v>
+      </c>
+      <c r="C129" t="str">
+        <f>IF(D129=0,"",D129)</f>
+        <v/>
+      </c>
+      <c r="D129" cm="1">
+        <f t="array" ref="D129">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A129)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130">
+        <v>187</v>
+      </c>
+      <c r="C130" t="str">
+        <f>IF(D130=0,"",D130)</f>
+        <v/>
+      </c>
+      <c r="D130" cm="1">
+        <f t="array" ref="D130">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A130)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131">
+        <v>188</v>
+      </c>
+      <c r="C131" t="str">
+        <f>IF(D131=0,"",D131)</f>
+        <v/>
+      </c>
+      <c r="D131" cm="1">
+        <f t="array" ref="D131">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A131)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132">
+        <v>189</v>
+      </c>
+      <c r="C132" t="str">
+        <f>IF(D132=0,"",D132)</f>
+        <v/>
+      </c>
+      <c r="D132" cm="1">
+        <f t="array" ref="D132">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A132)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133">
+        <v>190</v>
+      </c>
+      <c r="C133" t="str">
+        <f>IF(D133=0,"",D133)</f>
+        <v/>
+      </c>
+      <c r="D133" cm="1">
+        <f t="array" ref="D133">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A133)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134">
+        <v>191</v>
+      </c>
+      <c r="D134" cm="1">
+        <f t="array" ref="D134">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A134)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135">
+        <v>192</v>
+      </c>
+      <c r="D135" cm="1">
+        <f t="array" ref="D135">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A135)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136">
+        <v>193</v>
+      </c>
+      <c r="D136" cm="1">
+        <f t="array" ref="D136">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A136)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137">
+        <v>194</v>
+      </c>
+      <c r="D137" cm="1">
+        <f t="array" ref="D137">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A137)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138">
+        <v>195</v>
+      </c>
+      <c r="D138" cm="1">
+        <f t="array" ref="D138">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A138)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139">
+        <v>196</v>
+      </c>
+      <c r="D139" cm="1">
+        <f t="array" ref="D139">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A139)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140">
+        <v>197</v>
+      </c>
+      <c r="D140" cm="1">
+        <f t="array" ref="D140">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A140)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141">
+        <v>198</v>
+      </c>
+      <c r="D141" cm="1">
+        <f t="array" ref="D141">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A141)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142">
+        <v>199</v>
+      </c>
+      <c r="D142" cm="1">
+        <f t="array" ref="D142">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A142)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143">
+        <v>200</v>
+      </c>
+      <c r="D143" cm="1">
+        <f t="array" ref="D143">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A143)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144">
+        <v>201</v>
+      </c>
+      <c r="D144" cm="1">
+        <f t="array" ref="D144">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A144)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145">
+        <v>202</v>
+      </c>
+      <c r="D145" cm="1">
+        <f t="array" ref="D145">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A145)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146">
+        <v>203</v>
+      </c>
+      <c r="D146" cm="1">
+        <f t="array" ref="D146">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A146)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147">
+        <v>204</v>
+      </c>
+      <c r="D147" cm="1">
+        <f t="array" ref="D147">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A147)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148">
+        <v>205</v>
+      </c>
+      <c r="D148" cm="1">
+        <f t="array" ref="D148">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A148)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149">
+        <v>206</v>
+      </c>
+      <c r="D149" cm="1">
+        <f t="array" ref="D149">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A149)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150">
+        <v>207</v>
+      </c>
+      <c r="D150" cm="1">
+        <f t="array" ref="D150">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A150)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151">
+        <v>208</v>
+      </c>
+      <c r="D151" cm="1">
+        <f t="array" ref="D151">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A151)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152">
+        <v>209</v>
+      </c>
+      <c r="D152" cm="1">
+        <f t="array" ref="D152">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A152)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153">
+        <v>210</v>
+      </c>
+      <c r="D153" cm="1">
+        <f t="array" ref="D153">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A153)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154">
+        <v>211</v>
+      </c>
+      <c r="D154" cm="1">
+        <f t="array" ref="D154">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A154)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155">
+        <v>212</v>
+      </c>
+      <c r="D155" cm="1">
+        <f t="array" ref="D155">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A155)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156">
+        <v>213</v>
+      </c>
+      <c r="D156" cm="1">
+        <f t="array" ref="D156">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A156)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157">
+        <v>214</v>
+      </c>
+      <c r="D157" cm="1">
+        <f t="array" ref="D157">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A157)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158">
+        <v>215</v>
+      </c>
+      <c r="D158" cm="1">
+        <f t="array" ref="D158">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A158)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159">
+        <v>216</v>
+      </c>
+      <c r="D159" cm="1">
+        <f t="array" ref="D159">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A159)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160">
+        <v>217</v>
+      </c>
+      <c r="D160" cm="1">
+        <f t="array" ref="D160">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A160)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161">
+        <v>218</v>
+      </c>
+      <c r="D161" cm="1">
+        <f t="array" ref="D161">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A161)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162">
+        <v>219</v>
+      </c>
+      <c r="D162" cm="1">
+        <f t="array" ref="D162">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A162)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163">
+        <v>220</v>
+      </c>
+      <c r="D163" cm="1">
+        <f t="array" ref="D163">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A163)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164">
+        <v>221</v>
+      </c>
+      <c r="D164" cm="1">
+        <f t="array" ref="D164">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A164)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165">
+        <v>222</v>
+      </c>
+      <c r="D165" cm="1">
+        <f t="array" ref="D165">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A165)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166">
+        <v>223</v>
+      </c>
+      <c r="D166" cm="1">
+        <f t="array" ref="D166">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A166)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167">
+        <v>224</v>
+      </c>
+      <c r="D167" cm="1">
+        <f t="array" ref="D167">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A167)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168">
+        <v>225</v>
+      </c>
+      <c r="D168" cm="1">
+        <f t="array" ref="D168">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A168)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169">
+        <v>226</v>
+      </c>
+      <c r="D169" cm="1">
+        <f t="array" ref="D169">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A169)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170">
+        <v>227</v>
+      </c>
+      <c r="D170" cm="1">
+        <f t="array" ref="D170">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A170)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171">
+        <v>228</v>
+      </c>
+      <c r="D171" cm="1">
+        <f t="array" ref="D171">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A171)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172">
+        <v>229</v>
+      </c>
+      <c r="D172" cm="1">
+        <f t="array" ref="D172">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A172)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173">
+        <v>230</v>
+      </c>
+      <c r="D173" cm="1">
+        <f t="array" ref="D173">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A173)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174">
+        <v>231</v>
+      </c>
+      <c r="D174" cm="1">
+        <f t="array" ref="D174">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A174)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175">
+        <v>232</v>
+      </c>
+      <c r="D175" cm="1">
+        <f t="array" ref="D175">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A175)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176">
+        <v>233</v>
+      </c>
+      <c r="D176" cm="1">
+        <f t="array" ref="D176">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A176)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177">
+        <v>234</v>
+      </c>
+      <c r="D177" cm="1">
+        <f t="array" ref="D177">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A177)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178">
+        <v>235</v>
+      </c>
+      <c r="D178" cm="1">
+        <f t="array" ref="D178">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A178)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179">
+        <v>236</v>
+      </c>
+      <c r="D179" cm="1">
+        <f t="array" ref="D179">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A179)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180">
+        <v>237</v>
+      </c>
+      <c r="D180" cm="1">
+        <f t="array" ref="D180">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A180)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181">
+        <v>238</v>
+      </c>
+      <c r="D181" cm="1">
+        <f t="array" ref="D181">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A181)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182">
+        <v>239</v>
+      </c>
+      <c r="D182" cm="1">
+        <f t="array" ref="D182">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A182)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183">
+        <v>240</v>
+      </c>
+      <c r="D183" cm="1">
+        <f t="array" ref="D183">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A183)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184">
+        <v>241</v>
+      </c>
+      <c r="D184" cm="1">
+        <f t="array" ref="D184">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A184)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185">
+        <v>242</v>
+      </c>
+      <c r="D185" cm="1">
+        <f t="array" ref="D185">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A185)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186">
+        <v>243</v>
+      </c>
+      <c r="D186" cm="1">
+        <f t="array" ref="D186">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A186)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187">
+        <v>244</v>
+      </c>
+      <c r="D187" cm="1">
+        <f t="array" ref="D187">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A187)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188">
+        <v>245</v>
+      </c>
+      <c r="D188" cm="1">
+        <f t="array" ref="D188">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A188)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189">
+        <v>246</v>
+      </c>
+      <c r="D189" cm="1">
+        <f t="array" ref="D189">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A189)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190">
+        <v>247</v>
+      </c>
+      <c r="D190" cm="1">
+        <f t="array" ref="D190">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A190)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191">
+        <v>248</v>
+      </c>
+      <c r="D191" cm="1">
+        <f t="array" ref="D191">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A191)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192">
+        <v>249</v>
+      </c>
+      <c r="D192" cm="1">
+        <f t="array" ref="D192">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A192)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193">
+        <v>250</v>
+      </c>
+      <c r="D193" cm="1">
+        <f t="array" ref="D193">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A193)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194">
+        <v>251</v>
+      </c>
+      <c r="D194" cm="1">
+        <f t="array" ref="D194">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A194)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195">
+        <v>252</v>
+      </c>
+      <c r="D195" cm="1">
+        <f t="array" ref="D195">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A195)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196">
+        <v>253</v>
+      </c>
+      <c r="D196" cm="1">
+        <f t="array" ref="D196">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A196)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197">
+        <v>254</v>
+      </c>
+      <c r="D197" cm="1">
+        <f t="array" ref="D197">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A197)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198">
+        <v>255</v>
+      </c>
+      <c r="D198" cm="1">
+        <f t="array" ref="D198">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A198)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199">
+        <v>256</v>
+      </c>
+      <c r="D199" cm="1">
+        <f t="array" ref="D199">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A199)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200">
+        <v>257</v>
+      </c>
+      <c r="D200" cm="1">
+        <f t="array" ref="D200">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A200)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201">
+        <v>258</v>
+      </c>
+      <c r="D201" cm="1">
+        <f t="array" ref="D201">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A201)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202">
+        <v>259</v>
+      </c>
+      <c r="D202" cm="1">
+        <f t="array" ref="D202">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A202)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203">
+        <v>260</v>
+      </c>
+      <c r="D203" cm="1">
+        <f t="array" ref="D203">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A203)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204">
+        <v>261</v>
+      </c>
+      <c r="D204" cm="1">
+        <f t="array" ref="D204">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A204)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205">
+        <v>262</v>
+      </c>
+      <c r="D205" cm="1">
+        <f t="array" ref="D205">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A205)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206">
+        <v>263</v>
+      </c>
+      <c r="D206" cm="1">
+        <f t="array" ref="D206">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A206)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207">
+        <v>264</v>
+      </c>
+      <c r="D207" cm="1">
+        <f t="array" ref="D207">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A207)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208">
+        <v>265</v>
+      </c>
+      <c r="D208" cm="1">
+        <f t="array" ref="D208">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A208)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209">
+        <v>266</v>
+      </c>
+      <c r="D209" cm="1">
+        <f t="array" ref="D209">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A209)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210">
+        <v>267</v>
+      </c>
+      <c r="D210" cm="1">
+        <f t="array" ref="D210">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A210)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211">
+        <v>268</v>
+      </c>
+      <c r="D211" cm="1">
+        <f t="array" ref="D211">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A211)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212">
+        <v>269</v>
+      </c>
+      <c r="D212" cm="1">
+        <f t="array" ref="D212">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A212)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213">
+        <v>270</v>
+      </c>
+      <c r="D213" cm="1">
+        <f t="array" ref="D213">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A213)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214">
+        <v>271</v>
+      </c>
+      <c r="D214" cm="1">
+        <f t="array" ref="D214">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A214)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215">
+        <v>272</v>
+      </c>
+      <c r="D215" cm="1">
+        <f t="array" ref="D215">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A215)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216">
+        <v>273</v>
+      </c>
+      <c r="D216" cm="1">
+        <f t="array" ref="D216">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A216)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217">
+        <v>274</v>
+      </c>
+      <c r="D217" cm="1">
+        <f t="array" ref="D217">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A217)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218">
+        <v>275</v>
+      </c>
+      <c r="D218" cm="1">
+        <f t="array" ref="D218">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A218)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219">
+        <v>276</v>
+      </c>
+      <c r="D219" cm="1">
+        <f t="array" ref="D219">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A219)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220">
+        <v>277</v>
+      </c>
+      <c r="D220" cm="1">
+        <f t="array" ref="D220">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A220)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221">
+        <v>278</v>
+      </c>
+      <c r="D221" cm="1">
+        <f t="array" ref="D221">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A221)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222">
+        <v>279</v>
+      </c>
+      <c r="D222" cm="1">
+        <f t="array" ref="D222">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A222)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223">
+        <v>280</v>
+      </c>
+      <c r="D223" cm="1">
+        <f t="array" ref="D223">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A223)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224">
+        <v>281</v>
+      </c>
+      <c r="D224" cm="1">
+        <f t="array" ref="D224">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A224)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225">
+        <v>282</v>
+      </c>
+      <c r="D225" cm="1">
+        <f t="array" ref="D225">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A225)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226">
+        <v>283</v>
+      </c>
+      <c r="D226" cm="1">
+        <f t="array" ref="D226">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A226)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227">
+        <v>284</v>
+      </c>
+      <c r="D227" cm="1">
+        <f t="array" ref="D227">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A227)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228">
+        <v>285</v>
+      </c>
+      <c r="D228" cm="1">
+        <f t="array" ref="D228">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A228)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229">
+        <v>286</v>
+      </c>
+      <c r="D229" cm="1">
+        <f t="array" ref="D229">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A229)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A230">
+        <v>287</v>
+      </c>
+      <c r="D230" cm="1">
+        <f t="array" ref="D230">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A230)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A231">
+        <v>288</v>
+      </c>
+      <c r="D231" cm="1">
+        <f t="array" ref="D231">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A231)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A232">
+        <v>289</v>
+      </c>
+      <c r="D232" cm="1">
+        <f t="array" ref="D232">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A232)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A233">
+        <v>290</v>
+      </c>
+      <c r="D233" cm="1">
+        <f t="array" ref="D233">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A233)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A234">
+        <v>291</v>
+      </c>
+      <c r="D234" cm="1">
+        <f t="array" ref="D234">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A234)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A235">
+        <v>292</v>
+      </c>
+      <c r="D235" cm="1">
+        <f t="array" ref="D235">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A235)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A236">
+        <v>293</v>
+      </c>
+      <c r="D236" cm="1">
+        <f t="array" ref="D236">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A236)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237">
+        <v>294</v>
+      </c>
+      <c r="D237" cm="1">
+        <f t="array" ref="D237">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A237)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238">
+        <v>295</v>
+      </c>
+      <c r="D238" cm="1">
+        <f t="array" ref="D238">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A238)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239">
+        <v>296</v>
+      </c>
+      <c r="D239" cm="1">
+        <f t="array" ref="D239">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A239)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A240">
+        <v>297</v>
+      </c>
+      <c r="D240" cm="1">
+        <f t="array" ref="D240">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A240)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241">
+        <v>298</v>
+      </c>
+      <c r="D241" cm="1">
+        <f t="array" ref="D241">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A241)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242">
+        <v>299</v>
+      </c>
+      <c r="D242" cm="1">
+        <f t="array" ref="D242">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A242)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A243">
+        <v>300</v>
+      </c>
+      <c r="D243" cm="1">
+        <f t="array" ref="D243">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A243)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244">
+        <v>301</v>
+      </c>
+      <c r="D244" cm="1">
+        <f t="array" ref="D244">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A244)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A245">
+        <v>302</v>
+      </c>
+      <c r="D245" cm="1">
+        <f t="array" ref="D245">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A245)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A246">
+        <v>303</v>
+      </c>
+      <c r="D246" cm="1">
+        <f t="array" ref="D246">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A246)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A247">
+        <v>304</v>
+      </c>
+      <c r="D247" cm="1">
+        <f t="array" ref="D247">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A247)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248">
+        <v>305</v>
+      </c>
+      <c r="D248" cm="1">
+        <f t="array" ref="D248">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A248)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249">
+        <v>306</v>
+      </c>
+      <c r="D249" cm="1">
+        <f t="array" ref="D249">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A249)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250">
+        <v>307</v>
+      </c>
+      <c r="D250" cm="1">
+        <f t="array" ref="D250">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A250)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251">
+        <v>308</v>
+      </c>
+      <c r="D251" cm="1">
+        <f t="array" ref="D251">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A251)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252">
+        <v>309</v>
+      </c>
+      <c r="D252" cm="1">
+        <f t="array" ref="D252">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A252)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253">
+        <v>310</v>
+      </c>
+      <c r="D253" cm="1">
+        <f t="array" ref="D253">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A253)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254">
+        <v>311</v>
+      </c>
+      <c r="D254" cm="1">
+        <f t="array" ref="D254">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A254)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255">
+        <v>312</v>
+      </c>
+      <c r="D255" cm="1">
+        <f t="array" ref="D255">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A255)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256">
+        <v>313</v>
+      </c>
+      <c r="D256" cm="1">
+        <f t="array" ref="D256">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A256)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257">
+        <v>314</v>
+      </c>
+      <c r="D257" cm="1">
+        <f t="array" ref="D257">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A257)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258">
+        <v>315</v>
+      </c>
+      <c r="D258" cm="1">
+        <f t="array" ref="D258">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A258)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A259">
+        <v>316</v>
+      </c>
+      <c r="D259" cm="1">
+        <f t="array" ref="D259">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A259)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A260">
+        <v>317</v>
+      </c>
+      <c r="D260" cm="1">
+        <f t="array" ref="D260">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A260)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261">
+        <v>318</v>
+      </c>
+      <c r="D261" cm="1">
+        <f t="array" ref="D261">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A261)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A262">
+        <v>319</v>
+      </c>
+      <c r="D262" cm="1">
+        <f t="array" ref="D262">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A262)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A263">
+        <v>320</v>
+      </c>
+      <c r="D263" cm="1">
+        <f t="array" ref="D263">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A263)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A264">
+        <v>321</v>
+      </c>
+      <c r="D264" cm="1">
+        <f t="array" ref="D264">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A264)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A265">
+        <v>322</v>
+      </c>
+      <c r="D265" cm="1">
+        <f t="array" ref="D265">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A265)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A266">
+        <v>323</v>
+      </c>
+      <c r="D266" cm="1">
+        <f t="array" ref="D266">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A266)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A267">
+        <v>324</v>
+      </c>
+      <c r="D267" cm="1">
+        <f t="array" ref="D267">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A267)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A268">
+        <v>325</v>
+      </c>
+      <c r="D268" cm="1">
+        <f t="array" ref="D268">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A268)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A269">
+        <v>326</v>
+      </c>
+      <c r="D269" cm="1">
+        <f t="array" ref="D269">MAX(INDEX((calSameImpression_twitter8_1!B$1:B$468=A269)*calSameImpression_twitter8_1!C$1:C$468,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A270">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A271">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A272">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A273">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>